<commit_message>
completed Excel data importer
</commit_message>
<xml_diff>
--- a/TestCasesDataSheet.xlsx
+++ b/TestCasesDataSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ApexC\eclipse-workspace\AutomatedRegressionTestingPOC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ApexC\_repos\AutomatedRegressionTestingPOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="47">
   <si>
     <t>Execution</t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>na</t>
-  </si>
-  <si>
-    <t>Business Line</t>
   </si>
   <si>
     <t>Username</t>
@@ -510,7 +507,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,7 +545,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -559,7 +556,7 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
@@ -585,7 +582,7 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
@@ -663,7 +660,7 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>2</v>
@@ -689,7 +686,7 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>1</v>
@@ -715,7 +712,7 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>2</v>
@@ -741,7 +738,7 @@
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>1</v>
@@ -779,7 +776,7 @@
         <v>11</v>
       </c>
       <c r="G10">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>1</v>
@@ -805,7 +802,7 @@
         <v>12</v>
       </c>
       <c r="G11">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>1</v>
@@ -821,7 +818,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,13 +830,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -847,10 +844,10 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -858,10 +855,10 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -869,10 +866,10 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -898,7 +895,7 @@
         <v>23</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -906,7 +903,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -914,7 +911,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -922,7 +919,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -949,7 +946,7 @@
         <v>23</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -957,7 +954,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -965,7 +962,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -973,7 +970,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -981,7 +978,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented logging tool for test results
</commit_message>
<xml_diff>
--- a/TestCasesDataSheet.xlsx
+++ b/TestCasesDataSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ApexC\_repos\AutomatedRegressionTestingPOC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ApexC\_repos\AutomatedRegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -507,7 +507,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,7 +559,7 @@
         <v>44</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>

</xml_diff>